<commit_message>
Bug fix, streamline, modify plots slightly, new features
Some general streamlining and minor bug fixes. Collapsed all user-input files into one spreadsheet.  Added % carbonate evolved and error on temperatures.
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noaha\Desktop\blimp_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noaha\Documents\GitHub\blimp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8CE86F-C6A3-45A2-AB38-E88CE406464B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AEBE40-9329-474A-A0DA-4C67C7A5E2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="1836" windowWidth="16500" windowHeight="9492" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Anchors" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Thresholds" sheetId="3" r:id="rId3"/>
-    <sheet name="Rename_remove" sheetId="4" r:id="rId4"/>
-    <sheet name="Defaults" sheetId="5" r:id="rId5"/>
+    <sheet name="Rename_by_UID" sheetId="4" r:id="rId4"/>
+    <sheet name="Names_to_change" sheetId="5" r:id="rId5"/>
+    <sheet name="Remove" sheetId="7" r:id="rId6"/>
+    <sheet name="Metadata" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Anchor</t>
   </si>
@@ -76,9 +78,6 @@
     <t>New_name</t>
   </si>
   <si>
-    <t>Remove</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -143,6 +142,24 @@
   </si>
   <si>
     <t>transducer_pressure_thresh</t>
+  </si>
+  <si>
+    <t>old_name</t>
+  </si>
+  <si>
+    <t>new_name</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Ex: 20200105 NTA determined that a leak on the CO block led to erroneous D47 values</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Mineralogy</t>
   </si>
 </sst>
 </file>
@@ -508,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851CBD33-92C1-489B-80B7-086839040FD4}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -537,7 +554,7 @@
         <v>0.20519999999999999</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -548,7 +565,7 @@
         <v>0.20849999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,7 +576,7 @@
         <v>0.61319999999999997</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -570,7 +587,7 @@
         <v>0.45050000000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -581,7 +598,7 @@
         <v>0.64090000000000003</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -592,7 +609,7 @@
         <v>0.51349999999999996</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -616,46 +633,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>1.00871</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>1.00926</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>1.009091</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313594B5-B9A1-4667-8855-C8BB6D6B9DD7}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -696,77 +713,77 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>0.10299999999999999</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
         <v>-1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -776,20 +793,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A9C19B-CF1F-4CD7-A681-68B1EF1D6A4B}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -797,10 +813,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -810,14 +823,86 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A01DD5F-70EC-40D9-ABEF-A571E5D59CE8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0DE891-59B5-4876-B69A-D646B6C3CFF2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>99999</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854383EE-6F4D-41E7-ACC9-E8D80A8BE6E8}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added common typos for anchors to names to change tab
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noaha\Documents\GitHub\blimp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AEBE40-9329-474A-A0DA-4C67C7A5E2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5612F0-1AA7-45DE-AD2B-8CB89F12307A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Anchors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>Anchor</t>
   </si>
@@ -160,6 +160,117 @@
   </si>
   <si>
     <t>Mineralogy</t>
+  </si>
+  <si>
+    <t>ETH-01</t>
+  </si>
+  <si>
+    <t>ETH01</t>
+  </si>
+  <si>
+    <t>ETH1</t>
+  </si>
+  <si>
+    <t>ETH_01</t>
+  </si>
+  <si>
+    <t>ETH-02</t>
+  </si>
+  <si>
+    <t>ETH02</t>
+  </si>
+  <si>
+    <t>ETH2</t>
+  </si>
+  <si>
+    <t>ETH_02</t>
+  </si>
+  <si>
+    <t>ETH-03</t>
+  </si>
+  <si>
+    <t>ETH03</t>
+  </si>
+  <si>
+    <t>ETH3</t>
+  </si>
+  <si>
+    <t>ETH_03</t>
+  </si>
+  <si>
+    <t>ETH-04</t>
+  </si>
+  <si>
+    <t>ETH04</t>
+  </si>
+  <si>
+    <t>ETH4</t>
+  </si>
+  <si>
+    <t>ETH_04</t>
+  </si>
+  <si>
+    <t>IACA-C1</t>
+  </si>
+  <si>
+    <t>IAEA-C1</t>
+  </si>
+  <si>
+    <t>IAEAC1</t>
+  </si>
+  <si>
+    <t>IAEAC2</t>
+  </si>
+  <si>
+    <t>MERCK STD</t>
+  </si>
+  <si>
+    <t>Merck</t>
+  </si>
+  <si>
+    <t>Merck STD</t>
+  </si>
+  <si>
+    <t>Rodolo Dolomite</t>
+  </si>
+  <si>
+    <t>RODOLO</t>
+  </si>
+  <si>
+    <t>Rodolo</t>
+  </si>
+  <si>
+    <t>RODOLO DOLOMITE</t>
+  </si>
+  <si>
+    <t>Sansa Dolomite</t>
+  </si>
+  <si>
+    <t>SANSA</t>
+  </si>
+  <si>
+    <t>Sansa</t>
+  </si>
+  <si>
+    <t>SANSA DOLOMITE</t>
+  </si>
+  <si>
+    <t>TV-03</t>
+  </si>
+  <si>
+    <t>TV-04</t>
+  </si>
+  <si>
+    <t>EHT-01</t>
+  </si>
+  <si>
+    <t>EHT-02</t>
+  </si>
+  <si>
+    <t>EHT-03</t>
+  </si>
+  <si>
+    <t>EHT-04</t>
   </si>
 </sst>
 </file>
@@ -694,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313594B5-B9A1-4667-8855-C8BB6D6B9DD7}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -823,10 +934,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A01DD5F-70EC-40D9-ABEF-A571E5D59CE8}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,6 +952,270 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added T and d18Ow of each analysis
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noaha\Documents\GitHub\blimp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5612F0-1AA7-45DE-AD2B-8CB89F12307A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55909976-A5C7-4BDF-AA74-760583934ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
+    <workbookView xWindow="4212" yWindow="4212" windowWidth="14952" windowHeight="8712" firstSheet="3" activeTab="6" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Anchors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Anchor</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>EHT-04</t>
+  </si>
+  <si>
+    <t>SRM-88b</t>
+  </si>
+  <si>
+    <t>Dolomite</t>
   </si>
 </sst>
 </file>
@@ -936,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A01DD5F-70EC-40D9-ABEF-A571E5D59CE8}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B34"/>
     </sheetView>
   </sheetViews>
@@ -1257,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854383EE-6F4D-41E7-ACC9-E8D80A8BE6E8}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,6 +1283,14 @@
         <v>39</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed folder reading bug
Fixed bug where recently updated data folders were not being read in to blimp_main because DS Store was being read first and the loop was broken.
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noaha\Documents\GitHub\blimp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4E153-A6DD-4E30-AC49-5173E5B680F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20BA193-6EAB-4636-85BE-B97EB6613FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4956" yWindow="14172" windowWidth="15360" windowHeight="9516" firstSheet="1" activeTab="6" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{449AC5F2-A593-4BA4-BD07-2CD1BA0C4AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Anchors" sheetId="1" r:id="rId1"/>
@@ -664,13 +664,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -681,7 +681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -692,7 +692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -703,7 +703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -714,7 +714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -725,7 +725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -736,7 +736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -760,13 +760,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -777,7 +777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -788,7 +788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -799,7 +799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -810,12 +810,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -833,14 +833,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="67.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="67.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -854,7 +854,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -868,7 +868,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -896,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -910,7 +910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -938,7 +938,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
     </row>
@@ -956,13 +956,13 @@
       <selection activeCell="C4" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -982,17 +982,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A01DD5F-70EC-40D9-ABEF-A571E5D59CE8}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="A35:B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="2" width="29.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1264,167 +1264,167 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
     </row>
   </sheetData>
@@ -1441,9 +1441,9 @@
       <selection activeCell="A3" sqref="A3:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>99999</v>
       </c>
@@ -1469,17 +1469,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854383EE-6F4D-41E7-ACC9-E8D80A8BE6E8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>

</xml_diff>